<commit_message>
fix: adjust vertical positioning in wellcome_card function
</commit_message>
<xml_diff>
--- a/Docs/sociosExample.xlsx
+++ b/Docs/sociosExample.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Carlos</t>
+          <t>Carlos Francisco</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Juan Miguel</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">

</xml_diff>